<commit_message>
revisão final planilha financeira
</commit_message>
<xml_diff>
--- a/DOCS/Planilha Financeira de Custos.xlsx
+++ b/DOCS/Planilha Financeira de Custos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4632" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="0 - CONFIG" sheetId="9" r:id="rId1"/>
@@ -19,19 +19,26 @@
     <sheet name="4 - CT" sheetId="5" r:id="rId5"/>
     <sheet name="5 - CG" sheetId="7" r:id="rId6"/>
     <sheet name="6 - PF" sheetId="8" r:id="rId7"/>
+    <sheet name="7 - IT" sheetId="10" r:id="rId8"/>
+    <sheet name="8 - DRE" sheetId="11" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="INVESTIMENTO_TOTAL">'7 - IT'!$C$3</definedName>
     <definedName name="ISS">'0 - CONFIG'!$B$2</definedName>
-    <definedName name="QTD_TICKET_MES">'0 - CONFIG'!$B$5</definedName>
+    <definedName name="LUCRO_LIQUIDO">'7 - IT'!$C$10</definedName>
+    <definedName name="MARGEM_CONTRIBUICAO">'7 - IT'!$C$7</definedName>
+    <definedName name="MEDIA_TICKET">'0 - CONFIG'!$B$5</definedName>
+    <definedName name="QTD_TICKET_MES">'0 - CONFIG'!$B$3</definedName>
     <definedName name="SALARIO_PROGRAMADOR">'2 - CF'!$C$4</definedName>
-    <definedName name="TAXA_INSCRICAO">'0 - CONFIG'!$B$6</definedName>
-    <definedName name="TAXA_SERVICO">'0 - CONFIG'!$B$4</definedName>
-    <definedName name="TEMPO_DESENVOLVIMENTO">'0 - CONFIG'!$B$7</definedName>
-    <definedName name="TICKET_MEDIO">'0 - CONFIG'!$B$3</definedName>
+    <definedName name="TAXA_INSCRICAO">'0 - CONFIG'!#REF!</definedName>
+    <definedName name="TAXA_SERVICO">'0 - CONFIG'!#REF!</definedName>
+    <definedName name="TEMPO_DESENVOLVIMENTO">'0 - CONFIG'!$B$4</definedName>
+    <definedName name="TICKET_MEDIO">'0 - CONFIG'!#REF!</definedName>
     <definedName name="TOTAL_CF">'2 - CF'!$D$17</definedName>
     <definedName name="TOTAL_CG">'5 - CG'!$D$17</definedName>
     <definedName name="TOTAL_CT">'4 - CT'!$D$17</definedName>
     <definedName name="TOTAL_CV">'3 - CV'!$D$17</definedName>
+    <definedName name="TOTAL_FATURAMENTO">'6 - PF'!$D$17</definedName>
     <definedName name="TOTAL_II">'1 - II'!$D$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -39,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
   <si>
     <t>IPTU</t>
   </si>
@@ -101,9 +108,6 @@
     <t>ISS</t>
   </si>
   <si>
-    <t>ISS (15%)</t>
-  </si>
-  <si>
     <t>INVESTIMENTO INICIAL</t>
   </si>
   <si>
@@ -146,38 +150,72 @@
     <t>VALOR</t>
   </si>
   <si>
-    <t>TAXA SOBRE SERVIÇO</t>
-  </si>
-  <si>
-    <t>TAXA SOBRE INSCRIÇÃO</t>
-  </si>
-  <si>
-    <t>TICKET MÉDIO</t>
-  </si>
-  <si>
-    <t>QTD SERVIÇOS MÊS</t>
-  </si>
-  <si>
-    <t>TAXA SOBRE INSCRIÇÃO (MÊS)</t>
-  </si>
-  <si>
-    <t>TAXA SOBRE SERVIÇO (MÊS)</t>
-  </si>
-  <si>
     <t>DESENVOLVIMENTO (6 MESES) - WEB + APP</t>
   </si>
   <si>
     <t>TEMPO DESENVOLVIMENTO (MESES)</t>
+  </si>
+  <si>
+    <t>INVESTIMENTO TOTAL</t>
+  </si>
+  <si>
+    <t>FATURAMENTO</t>
+  </si>
+  <si>
+    <t>CUSTO VARIÁVEL</t>
+  </si>
+  <si>
+    <t>MARGEM C.</t>
+  </si>
+  <si>
+    <t>CUSTO FIXO</t>
+  </si>
+  <si>
+    <t>LUCRO LIQUIDO</t>
+  </si>
+  <si>
+    <t>INDICADOR FINANCEIRO</t>
+  </si>
+  <si>
+    <t>ISS (5%)</t>
+  </si>
+  <si>
+    <t>PUBLICIDADE NO SITE (MÊS)</t>
+  </si>
+  <si>
+    <t>QTD PUBLICIDADE MÊS</t>
+  </si>
+  <si>
+    <t>TAXA RETORNO</t>
+  </si>
+  <si>
+    <t>VALOR MÉDIO DA PUBLICIDADE</t>
+  </si>
+  <si>
+    <t>MARGEM CONTRIBUIÇÃO</t>
+  </si>
+  <si>
+    <t>DEMONSTRAÇÃO DE RESULTADO (DRE)</t>
+  </si>
+  <si>
+    <t>LUCRATIVIDADE</t>
+  </si>
+  <si>
+    <t>RENTABILIDADE</t>
+  </si>
+  <si>
+    <t>LUCRO LÍQUIDO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -210,8 +248,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,11 +299,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -264,15 +315,42 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,16 +662,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,64 +687,44 @@
         <v>19</v>
       </c>
       <c r="B2" s="2">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.2</v>
+      <c r="B4" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1000</v>
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4">
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="12">
-        <v>100</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="4">
-        <v>6</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -678,23 +736,23 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -704,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -835,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6">
         <f>SALARIO_PROGRAMADOR*TEMPO_DESENVOLVIMENTO</f>
@@ -926,18 +984,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -947,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -958,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6">
         <v>3500</v>
@@ -973,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6">
         <v>1500</v>
@@ -988,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="6">
         <v>1500</v>
@@ -1018,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6">
         <v>200</v>
@@ -1063,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6">
         <v>50</v>
@@ -1078,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="6">
         <v>100</v>
@@ -1161,23 +1219,23 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1187,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -1219,25 +1277,25 @@
         <v>600</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D6" si="0">C5*A5</f>
+        <f t="shared" ref="D5" si="0">C5*A5</f>
         <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>QTD_TICKET_MES</f>
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C6" s="6">
-        <f>TICKET_MEDIO</f>
-        <v>100</v>
+        <f>MEDIA_TICKET</f>
+        <v>500</v>
       </c>
       <c r="D6" s="6">
         <f>C6*A6*ISS</f>
-        <v>15000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1305,11 +1363,11 @@
       <c r="B17" s="8"/>
       <c r="C17" s="9">
         <f>SUM(C4:C16)</f>
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="D17" s="9">
         <f>SUM(D4:D16)</f>
-        <v>16200</v>
+        <v>3700</v>
       </c>
     </row>
   </sheetData>
@@ -1325,23 +1383,23 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1351,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -1362,14 +1420,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6">
         <f>TOTAL_CF</f>
         <v>14450</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D16" si="0">C4*A4</f>
+        <f t="shared" ref="D4:D6" si="0">C4*A4</f>
         <v>14450</v>
       </c>
     </row>
@@ -1378,15 +1436,15 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6">
         <f>TOTAL_CV</f>
-        <v>16200</v>
+        <v>3700</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>16200</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1493,11 +1551,11 @@
       <c r="B17" s="8"/>
       <c r="C17" s="9">
         <f>SUM(C4:C16)</f>
-        <v>30650</v>
+        <v>18150</v>
       </c>
       <c r="D17" s="9">
         <f>SUM(D4:D16)</f>
-        <v>30650</v>
+        <v>18150</v>
       </c>
     </row>
   </sheetData>
@@ -1513,23 +1571,23 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1539,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -1550,15 +1608,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6">
         <f>TOTAL_CT</f>
-        <v>30650</v>
+        <v>18150</v>
       </c>
       <c r="D4" s="6">
         <f>C4*A4</f>
-        <v>91950</v>
+        <v>54450</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,11 +1732,194 @@
       <c r="B17" s="8"/>
       <c r="C17" s="9">
         <f>SUM(C4:C16)</f>
-        <v>30650</v>
+        <v>18150</v>
       </c>
       <c r="D17" s="9">
         <f>SUM(D4:D16)</f>
-        <v>91950</v>
+        <v>54450</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>QTD_TICKET_MES</f>
+        <v>100</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="6">
+        <f>MEDIA_TICKET</f>
+        <v>500</v>
+      </c>
+      <c r="D4" s="6">
+        <f>C4*A4</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:D16" si="0">C5*A5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9">
+        <f>SUM(C4:C16)</f>
+        <v>500</v>
+      </c>
+      <c r="D17" s="9">
+        <f>SUM(D4:D16)</f>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -1689,191 +1930,238 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="3" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f>QTD_TICKET_MES</f>
-        <v>1000</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <f>TOTAL_II</f>
+        <v>57650</v>
+      </c>
+      <c r="B3" s="15">
+        <f>TOTAL_CG</f>
+        <v>54450</v>
+      </c>
+      <c r="C3" s="15">
+        <f>SUM(A3+B3)</f>
+        <v>112100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <f>TOTAL_FATURAMENTO</f>
+        <v>50000</v>
+      </c>
+      <c r="B7" s="17">
+        <f>TOTAL_CV</f>
+        <v>3700</v>
+      </c>
+      <c r="C7" s="17">
+        <f>A7-B7</f>
+        <v>46300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="6">
-        <f>TICKET_MEDIO*TAXA_SERVICO</f>
-        <v>20</v>
-      </c>
-      <c r="D4" s="6">
-        <f>C4*A4</f>
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>100</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6">
-        <f>TAXA_INSCRICAO</f>
-        <v>100</v>
-      </c>
-      <c r="D5" s="6">
-        <f t="shared" ref="D5:D16" si="0">C5*A5</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9">
-        <f>SUM(C4:C16)</f>
-        <v>120</v>
-      </c>
-      <c r="D17" s="9">
-        <f>SUM(D4:D16)</f>
-        <v>30000</v>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <f>MARGEM_CONTRIBUICAO</f>
+        <v>46300</v>
+      </c>
+      <c r="B10" s="17">
+        <f>TOTAL_CF</f>
+        <v>14450</v>
+      </c>
+      <c r="C10" s="17">
+        <f>A10-B10</f>
+        <v>31850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <f>LUCRO_LIQUIDO</f>
+        <v>31850</v>
+      </c>
+      <c r="B14" s="19">
+        <f>TOTAL_FATURAMENTO</f>
+        <v>50000</v>
+      </c>
+      <c r="C14" s="20">
+        <f>A14/B14</f>
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <f>LUCRO_LIQUIDO</f>
+        <v>31850</v>
+      </c>
+      <c r="B17" s="19">
+        <f>INVESTIMENTO_TOTAL</f>
+        <v>112100</v>
+      </c>
+      <c r="C17" s="20">
+        <f>A17/B17</f>
+        <v>0.28412132024977699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <f>INVESTIMENTO_TOTAL</f>
+        <v>112100</v>
+      </c>
+      <c r="B20" s="19">
+        <f>LUCRO_LIQUIDO</f>
+        <v>31850</v>
+      </c>
+      <c r="C20" s="20">
+        <f>A20/B20</f>
+        <v>3.5196232339089484</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>